<commit_message>
add imputation of retirees and beneficiaries data
</commit_message>
<xml_diff>
--- a/Data/UCRP-MembersData-2015(1).xlsx
+++ b/Data/UCRP-MembersData-2015(1).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Active_t76 (2)" sheetId="21" r:id="rId1"/>
@@ -30,12 +30,12 @@
     <sheet name="Actives_tm13" sheetId="9" r:id="rId16"/>
     <sheet name="Actives_safety" sheetId="10" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="171027" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="141">
   <si>
     <t>&lt; 50</t>
   </si>
@@ -461,15 +461,58 @@
       <t>24</t>
     </r>
   </si>
+  <si>
+    <t>nretirees</t>
+  </si>
+  <si>
+    <t>benefit</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>70-74</t>
+  </si>
+  <si>
+    <t>75-79</t>
+  </si>
+  <si>
+    <t>80-84</t>
+  </si>
+  <si>
+    <t>85-89</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>benperiod</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>n.R0S1</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>name_N</t>
+  </si>
+  <si>
+    <t>name_V</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -558,7 +601,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -580,6 +623,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -657,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -790,38 +839,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -856,6 +878,67 @@
     </xf>
     <xf numFmtId="1" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -950,6 +1033,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -985,6 +1085,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1190,15 +1307,15 @@
       <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="68"/>
       <c r="H2" s="37"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
@@ -1218,13 +1335,13 @@
       <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="52"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="68"/>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
@@ -1236,10 +1353,10 @@
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
       <c r="D5" s="38"/>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="54"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="38"/>
       <c r="H5" s="38"/>
       <c r="I5" s="38"/>
@@ -2487,12 +2604,12 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2745,12 +2862,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
@@ -2926,273 +3043,636 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+    </row>
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="52"/>
+      <c r="G7" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="H7" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="I7" s="77" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="8" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="84" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="52"/>
+      <c r="G8" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="25">
+      <c r="H8" s="78">
         <v>5</v>
       </c>
-      <c r="C4" s="24">
+      <c r="I8" s="79">
         <v>910.12800000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="85">
+        <v>52</v>
+      </c>
+      <c r="D9" s="86">
+        <f>SUM(H8:H9)</f>
+        <v>553</v>
+      </c>
+      <c r="E9" s="86">
+        <f>(H8*I8+H9*I9)/SUM(H8:H9)</f>
+        <v>1650.3560940325497</v>
+      </c>
+      <c r="F9" s="52"/>
+      <c r="G9" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="25">
+      <c r="H9" s="78">
         <v>548</v>
       </c>
-      <c r="C5" s="24">
+      <c r="I9" s="79">
         <v>1657.11</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="85">
+        <v>57</v>
+      </c>
+      <c r="D10" s="86">
+        <v>2752</v>
+      </c>
+      <c r="E10" s="86">
+        <v>2455.81</v>
+      </c>
+      <c r="F10" s="79"/>
+      <c r="G10" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="25">
+      <c r="H10" s="78">
         <v>2752</v>
       </c>
-      <c r="C6" s="24">
+      <c r="I10" s="79">
         <v>2455.81</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="K10" s="81"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="85">
+        <v>62</v>
+      </c>
+      <c r="D11" s="86">
+        <v>9410</v>
+      </c>
+      <c r="E11" s="86">
+        <v>3195</v>
+      </c>
+      <c r="F11" s="79"/>
+      <c r="G11" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="25">
+      <c r="H11" s="78">
         <v>9410</v>
       </c>
-      <c r="C7" s="24">
+      <c r="I11" s="79">
         <v>3195</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="85">
+        <v>67</v>
+      </c>
+      <c r="D12" s="86">
+        <v>11989</v>
+      </c>
+      <c r="E12" s="86">
+        <v>3225.72</v>
+      </c>
+      <c r="F12" s="79"/>
+      <c r="G12" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="25">
+      <c r="H12" s="78">
         <v>11989</v>
       </c>
-      <c r="C8" s="24">
+      <c r="I12" s="79">
         <v>3225.72</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="85">
+        <v>72</v>
+      </c>
+      <c r="D13" s="86">
+        <v>8888</v>
+      </c>
+      <c r="E13" s="86">
+        <v>3522.88</v>
+      </c>
+      <c r="F13" s="79"/>
+      <c r="G13" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="25">
+      <c r="H13" s="78">
         <v>8888</v>
       </c>
-      <c r="C9" s="24">
+      <c r="I13" s="79">
         <v>3522.88</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="85">
+        <v>77</v>
+      </c>
+      <c r="D14" s="86">
+        <v>5651</v>
+      </c>
+      <c r="E14" s="86">
+        <v>3517.86</v>
+      </c>
+      <c r="F14" s="79"/>
+      <c r="G14" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="25">
+      <c r="H14" s="78">
         <v>5651</v>
       </c>
-      <c r="C10" s="24">
+      <c r="I14" s="79">
         <v>3517.86</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="85" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="85">
+        <v>82</v>
+      </c>
+      <c r="D15" s="86">
+        <v>3667</v>
+      </c>
+      <c r="E15" s="86">
+        <v>3478.87</v>
+      </c>
+      <c r="F15" s="79"/>
+      <c r="G15" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="25">
+      <c r="H15" s="78">
         <v>3667</v>
       </c>
-      <c r="C11" s="24">
+      <c r="I15" s="79">
         <v>3478.87</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="85" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="85">
+        <v>87</v>
+      </c>
+      <c r="D16" s="86">
+        <v>3506</v>
+      </c>
+      <c r="E16" s="86">
+        <v>3053.74</v>
+      </c>
+      <c r="F16" s="79"/>
+      <c r="G16" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="25">
+      <c r="H16" s="78">
         <v>3506</v>
       </c>
-      <c r="C12" s="24">
+      <c r="I16" s="79">
         <v>3053.74</v>
       </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F17" s="79"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F18" s="52"/>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F19" s="52"/>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F20" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>129</v>
+      </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D7" s="84" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="84" t="s">
+        <v>128</v>
+      </c>
+      <c r="G7" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="I7" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="82" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="82" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="25">
+      <c r="H8" s="25">
         <v>234</v>
       </c>
-      <c r="C4" s="24">
+      <c r="I8" s="24">
         <v>1346.87</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="85" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="85">
+        <v>52</v>
+      </c>
+      <c r="D9" s="86">
+        <f>SUM(H8:H9)</f>
+        <v>406</v>
+      </c>
+      <c r="E9" s="86">
+        <f>(H8*I8+H9*I9)/SUM(H8:H9)</f>
+        <v>1496.3786699507389</v>
+      </c>
+      <c r="G9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="25">
+      <c r="H9" s="25">
         <v>172</v>
       </c>
-      <c r="C5" s="24">
+      <c r="I9" s="24">
         <v>1699.78</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="85" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="85">
+        <v>57</v>
+      </c>
+      <c r="D10" s="80">
+        <v>318</v>
+      </c>
+      <c r="E10" s="80">
+        <v>1844.05</v>
+      </c>
+      <c r="G10" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="25">
+      <c r="H10" s="25">
         <v>318</v>
       </c>
-      <c r="C6" s="24">
+      <c r="I10" s="24">
         <v>1844.05</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="85">
+        <v>62</v>
+      </c>
+      <c r="D11" s="80">
+        <v>637</v>
+      </c>
+      <c r="E11" s="80">
+        <v>2020.73</v>
+      </c>
+      <c r="G11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="25">
+      <c r="H11" s="25">
         <v>637</v>
       </c>
-      <c r="C7" s="24">
+      <c r="I11" s="24">
         <v>2020.73</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="85">
+        <v>67</v>
+      </c>
+      <c r="D12" s="80">
+        <v>867</v>
+      </c>
+      <c r="E12" s="80">
+        <v>2175.9</v>
+      </c>
+      <c r="G12" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="25">
+      <c r="H12" s="25">
         <v>867</v>
       </c>
-      <c r="C8" s="24">
+      <c r="I12" s="24">
         <v>2175.9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="85">
+        <v>72</v>
+      </c>
+      <c r="D13" s="80">
+        <v>865</v>
+      </c>
+      <c r="E13" s="80">
+        <v>2516.38</v>
+      </c>
+      <c r="G13" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="25">
+      <c r="H13" s="25">
         <v>865</v>
       </c>
-      <c r="C9" s="24">
+      <c r="I13" s="24">
         <v>2516.38</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="85" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" s="85">
+        <v>77</v>
+      </c>
+      <c r="D14" s="80">
+        <v>825</v>
+      </c>
+      <c r="E14" s="80">
+        <v>2398.98</v>
+      </c>
+      <c r="G14" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="25">
+      <c r="H14" s="25">
         <v>825</v>
       </c>
-      <c r="C10" s="24">
+      <c r="I14" s="24">
         <v>2398.98</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="85" t="s">
+        <v>132</v>
+      </c>
+      <c r="C15" s="85">
+        <v>82</v>
+      </c>
+      <c r="D15" s="80">
+        <v>834</v>
+      </c>
+      <c r="E15" s="80">
+        <v>2298.7600000000002</v>
+      </c>
+      <c r="G15" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="25">
+      <c r="H15" s="25">
         <v>834</v>
       </c>
-      <c r="C11" s="24">
+      <c r="I15" s="24">
         <v>2298.7600000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="85" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="85">
+        <v>87</v>
+      </c>
+      <c r="D16" s="80">
+        <v>1366</v>
+      </c>
+      <c r="E16" s="80">
+        <v>2357.0700000000002</v>
+      </c>
+      <c r="G16" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="25">
+      <c r="H16" s="25">
         <v>1366</v>
       </c>
-      <c r="C12" s="24">
+      <c r="I16" s="24">
         <v>2357.0700000000002</v>
       </c>
     </row>
@@ -3205,1287 +3685,1287 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="60"/>
-    <col min="3" max="3" width="17.5703125" style="60" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="60"/>
-    <col min="5" max="6" width="9.140625" style="72"/>
-    <col min="7" max="10" width="14.85546875" style="60" customWidth="1"/>
-    <col min="11" max="15" width="13.7109375" style="60" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="60" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="60"/>
+    <col min="1" max="2" width="9.140625" style="52"/>
+    <col min="3" max="3" width="17.5703125" style="52" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="52"/>
+    <col min="5" max="6" width="9.140625" style="63"/>
+    <col min="7" max="10" width="14.85546875" style="52" customWidth="1"/>
+    <col min="11" max="15" width="13.7109375" style="52" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="52" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="52" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="52" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G6" s="58" t="s">
+      <c r="G6" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G7" s="67" t="s">
+      <c r="G7" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G8" s="68" t="s">
+      <c r="G8" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C9" s="58"/>
-      <c r="G9" s="58"/>
-      <c r="H9" s="58"/>
-      <c r="I9" s="58"/>
-      <c r="J9" s="61" t="s">
+      <c r="C9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="73" t="s">
         <v>48</v>
       </c>
-      <c r="K9" s="61"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
+      <c r="K9" s="73"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C10" s="58" t="s">
+      <c r="C10" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="62" t="s">
+      <c r="G10" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="H10" s="63" t="s">
+      <c r="H10" s="54" t="s">
         <v>99</v>
       </c>
-      <c r="I10" s="63" t="s">
+      <c r="I10" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="J10" s="62" t="s">
+      <c r="J10" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="62" t="s">
+      <c r="K10" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="L10" s="62" t="s">
+      <c r="L10" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="62" t="s">
+      <c r="M10" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="N10" s="62" t="s">
+      <c r="N10" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="O10" s="58" t="s">
+      <c r="O10" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="P10" s="58" t="s">
+      <c r="P10" s="50" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="71" t="s">
+      <c r="C11" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="F11" s="70" t="s">
+      <c r="F11" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="G11" s="70">
+      <c r="G11" s="61">
         <v>2</v>
       </c>
-      <c r="H11" s="70">
+      <c r="H11" s="61">
         <v>7</v>
       </c>
-      <c r="I11" s="70">
+      <c r="I11" s="61">
         <v>12</v>
       </c>
-      <c r="J11" s="70">
+      <c r="J11" s="61">
         <v>17</v>
       </c>
-      <c r="K11" s="70">
+      <c r="K11" s="61">
         <v>22</v>
       </c>
-      <c r="L11" s="70">
+      <c r="L11" s="61">
         <v>27</v>
       </c>
-      <c r="M11" s="70">
+      <c r="M11" s="61">
         <v>32</v>
       </c>
-      <c r="N11" s="70">
+      <c r="N11" s="61">
         <v>37</v>
       </c>
-      <c r="O11" s="70">
+      <c r="O11" s="61">
         <v>42</v>
       </c>
-      <c r="P11" s="58" t="s">
+      <c r="P11" s="50" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C12" s="71"/>
-      <c r="D12" s="70" t="s">
+      <c r="C12" s="62"/>
+      <c r="D12" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70" t="s">
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="61" t="s">
         <v>99</v>
       </c>
-      <c r="I12" s="70" t="s">
+      <c r="I12" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="70" t="s">
+      <c r="J12" s="61" t="s">
         <v>76</v>
       </c>
-      <c r="K12" s="70" t="s">
+      <c r="K12" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="L12" s="70" t="s">
+      <c r="L12" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="M12" s="70" t="s">
+      <c r="M12" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="N12" s="70" t="s">
+      <c r="N12" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="O12" s="70" t="s">
+      <c r="O12" s="61" t="s">
         <v>117</v>
       </c>
-      <c r="P12" s="58"/>
+      <c r="P12" s="50"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C13" s="62" t="s">
+      <c r="C13" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="69" t="s">
+      <c r="D13" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="73">
+      <c r="E13" s="64">
         <v>22</v>
       </c>
-      <c r="F13" s="73" t="s">
+      <c r="F13" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="G13" s="74">
+      <c r="G13" s="65">
         <v>450</v>
       </c>
-      <c r="H13" s="74">
+      <c r="H13" s="65">
         <v>16</v>
       </c>
-      <c r="I13" s="74" t="s">
+      <c r="I13" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="J13" s="74" t="s">
+      <c r="J13" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="K13" s="74" t="s">
+      <c r="K13" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="L13" s="74" t="s">
+      <c r="L13" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M13" s="74" t="s">
+      <c r="M13" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N13" s="74" t="s">
+      <c r="N13" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O13" s="74" t="s">
+      <c r="O13" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P13" s="62">
+      <c r="P13" s="53">
         <v>466</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="62"/>
-      <c r="D14" s="69" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E14" s="73">
+      <c r="E14" s="64">
         <v>22</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="F14" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="G14" s="74">
+      <c r="G14" s="65">
         <v>49125</v>
       </c>
-      <c r="H14" s="74">
+      <c r="H14" s="65">
         <v>42899</v>
       </c>
-      <c r="I14" s="74" t="s">
+      <c r="I14" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="J14" s="74" t="s">
+      <c r="J14" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="K14" s="74" t="s">
+      <c r="K14" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="L14" s="74" t="s">
+      <c r="L14" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M14" s="74" t="s">
+      <c r="M14" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N14" s="74" t="s">
+      <c r="N14" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O14" s="74" t="s">
+      <c r="O14" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P14" s="64">
+      <c r="P14" s="55">
         <v>48912</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="62" t="s">
+      <c r="C15" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="73">
+      <c r="E15" s="64">
         <v>27</v>
       </c>
-      <c r="F15" s="73" t="s">
+      <c r="F15" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="74">
+      <c r="G15" s="65">
         <v>4091</v>
       </c>
-      <c r="H15" s="74">
+      <c r="H15" s="65">
         <v>1113</v>
       </c>
-      <c r="I15" s="74">
+      <c r="I15" s="65">
         <v>18</v>
       </c>
-      <c r="J15" s="74" t="s">
+      <c r="J15" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="K15" s="74" t="s">
+      <c r="K15" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="L15" s="74" t="s">
+      <c r="L15" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M15" s="74" t="s">
+      <c r="M15" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N15" s="74" t="s">
+      <c r="N15" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O15" s="74" t="s">
+      <c r="O15" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P15" s="65">
+      <c r="P15" s="56">
         <v>5222</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C16" s="62"/>
-      <c r="D16" s="69" t="s">
+      <c r="C16" s="53"/>
+      <c r="D16" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="73">
+      <c r="E16" s="64">
         <v>27</v>
       </c>
-      <c r="F16" s="73" t="s">
+      <c r="F16" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="74">
+      <c r="G16" s="65">
         <v>62836</v>
       </c>
-      <c r="H16" s="74">
+      <c r="H16" s="65">
         <v>59637</v>
       </c>
-      <c r="I16" s="74">
+      <c r="I16" s="65">
         <v>46481</v>
       </c>
-      <c r="J16" s="74" t="s">
+      <c r="J16" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="K16" s="74" t="s">
+      <c r="K16" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="L16" s="74" t="s">
+      <c r="L16" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M16" s="74" t="s">
+      <c r="M16" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N16" s="74" t="s">
+      <c r="N16" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O16" s="74" t="s">
+      <c r="O16" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P16" s="65">
+      <c r="P16" s="56">
         <v>62098</v>
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="73">
+      <c r="E17" s="64">
         <v>32</v>
       </c>
-      <c r="F17" s="73" t="s">
+      <c r="F17" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="G17" s="74">
+      <c r="G17" s="65">
         <v>4579</v>
       </c>
-      <c r="H17" s="74">
+      <c r="H17" s="65">
         <v>4661</v>
       </c>
-      <c r="I17" s="74">
+      <c r="I17" s="65">
         <v>744</v>
       </c>
-      <c r="J17" s="74">
+      <c r="J17" s="65">
         <v>20</v>
       </c>
-      <c r="K17" s="74" t="s">
+      <c r="K17" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="L17" s="74" t="s">
+      <c r="L17" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M17" s="74" t="s">
+      <c r="M17" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N17" s="74" t="s">
+      <c r="N17" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O17" s="74" t="s">
+      <c r="O17" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P17" s="65">
+      <c r="P17" s="56">
         <v>10004</v>
       </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C18" s="62"/>
-      <c r="D18" s="69" t="s">
+      <c r="C18" s="53"/>
+      <c r="D18" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="73">
+      <c r="E18" s="64">
         <v>32</v>
       </c>
-      <c r="F18" s="73" t="s">
+      <c r="F18" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="G18" s="74">
+      <c r="G18" s="65">
         <v>77686</v>
       </c>
-      <c r="H18" s="74">
+      <c r="H18" s="65">
         <v>75964</v>
       </c>
-      <c r="I18" s="74">
+      <c r="I18" s="65">
         <v>66937</v>
       </c>
-      <c r="J18" s="74">
+      <c r="J18" s="65">
         <v>57202</v>
       </c>
-      <c r="K18" s="74" t="s">
+      <c r="K18" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="L18" s="74" t="s">
+      <c r="L18" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M18" s="74" t="s">
+      <c r="M18" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N18" s="74" t="s">
+      <c r="N18" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O18" s="74" t="s">
+      <c r="O18" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P18" s="65">
+      <c r="P18" s="56">
         <v>76044</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="69" t="s">
+      <c r="D19" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="73">
+      <c r="E19" s="64">
         <v>37</v>
       </c>
-      <c r="F19" s="73" t="s">
+      <c r="F19" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="G19" s="74">
+      <c r="G19" s="65">
         <v>4218</v>
       </c>
-      <c r="H19" s="74">
+      <c r="H19" s="65">
         <v>5198</v>
       </c>
-      <c r="I19" s="74">
+      <c r="I19" s="65">
         <v>2558</v>
       </c>
-      <c r="J19" s="74">
+      <c r="J19" s="65">
         <v>514</v>
       </c>
-      <c r="K19" s="74">
+      <c r="K19" s="65">
         <v>6</v>
       </c>
-      <c r="L19" s="74" t="s">
+      <c r="L19" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M19" s="74" t="s">
+      <c r="M19" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N19" s="74" t="s">
+      <c r="N19" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O19" s="74" t="s">
+      <c r="O19" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P19" s="65">
+      <c r="P19" s="56">
         <v>12494</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C20" s="62"/>
-      <c r="D20" s="69" t="s">
+      <c r="C20" s="53"/>
+      <c r="D20" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="73">
+      <c r="E20" s="64">
         <v>37</v>
       </c>
-      <c r="F20" s="73" t="s">
+      <c r="F20" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="74">
+      <c r="G20" s="65">
         <v>88621</v>
       </c>
-      <c r="H20" s="74">
+      <c r="H20" s="65">
         <v>90614</v>
       </c>
-      <c r="I20" s="74">
+      <c r="I20" s="65">
         <v>80010</v>
       </c>
-      <c r="J20" s="74">
+      <c r="J20" s="65">
         <v>75111</v>
       </c>
-      <c r="K20" s="74">
+      <c r="K20" s="65">
         <v>77949</v>
       </c>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="M20" s="74" t="s">
+      <c r="M20" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N20" s="74" t="s">
+      <c r="N20" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O20" s="74" t="s">
+      <c r="O20" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P20" s="65">
+      <c r="P20" s="56">
         <v>87126</v>
       </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="D21" s="69" t="s">
+      <c r="D21" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="73">
+      <c r="E21" s="64">
         <v>42</v>
       </c>
-      <c r="F21" s="73" t="s">
+      <c r="F21" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="G21" s="74">
+      <c r="G21" s="65">
         <v>2898</v>
       </c>
-      <c r="H21" s="74">
+      <c r="H21" s="65">
         <v>5157</v>
       </c>
-      <c r="I21" s="74">
+      <c r="I21" s="65">
         <v>3656</v>
       </c>
-      <c r="J21" s="74">
+      <c r="J21" s="65">
         <v>1582</v>
       </c>
-      <c r="K21" s="74">
+      <c r="K21" s="65">
         <v>305</v>
       </c>
-      <c r="L21" s="74">
+      <c r="L21" s="65">
         <v>11</v>
       </c>
-      <c r="M21" s="74" t="s">
+      <c r="M21" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N21" s="74" t="s">
+      <c r="N21" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O21" s="74" t="s">
+      <c r="O21" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P21" s="65">
+      <c r="P21" s="56">
         <v>13609</v>
       </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C22" s="62"/>
-      <c r="D22" s="69" t="s">
+      <c r="C22" s="53"/>
+      <c r="D22" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E22" s="73">
+      <c r="E22" s="64">
         <v>42</v>
       </c>
-      <c r="F22" s="73" t="s">
+      <c r="F22" s="64" t="s">
         <v>112</v>
       </c>
-      <c r="G22" s="74">
+      <c r="G22" s="65">
         <v>89793</v>
       </c>
-      <c r="H22" s="74">
+      <c r="H22" s="65">
         <v>96293</v>
       </c>
-      <c r="I22" s="74">
+      <c r="I22" s="65">
         <v>95348</v>
       </c>
-      <c r="J22" s="74">
+      <c r="J22" s="65">
         <v>85513</v>
       </c>
-      <c r="K22" s="74">
+      <c r="K22" s="65">
         <v>81725</v>
       </c>
-      <c r="L22" s="74">
+      <c r="L22" s="65">
         <v>78205</v>
       </c>
-      <c r="M22" s="74" t="s">
+      <c r="M22" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="N22" s="74" t="s">
+      <c r="N22" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O22" s="74" t="s">
+      <c r="O22" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P22" s="65">
+      <c r="P22" s="56">
         <v>93061</v>
       </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="69" t="s">
+      <c r="D23" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E23" s="73">
+      <c r="E23" s="64">
         <v>47</v>
       </c>
-      <c r="F23" s="73" t="s">
+      <c r="F23" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="74">
+      <c r="G23" s="65">
         <v>2059</v>
       </c>
-      <c r="H23" s="74">
+      <c r="H23" s="65">
         <v>3911</v>
       </c>
-      <c r="I23" s="74">
+      <c r="I23" s="65">
         <v>3872</v>
       </c>
-      <c r="J23" s="74">
+      <c r="J23" s="65">
         <v>2416</v>
       </c>
-      <c r="K23" s="74">
+      <c r="K23" s="65">
         <v>1031</v>
       </c>
-      <c r="L23" s="74">
+      <c r="L23" s="65">
         <v>345</v>
       </c>
-      <c r="M23" s="74">
+      <c r="M23" s="65">
         <v>11</v>
       </c>
-      <c r="N23" s="74" t="s">
+      <c r="N23" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O23" s="74" t="s">
+      <c r="O23" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P23" s="65">
+      <c r="P23" s="56">
         <v>13645</v>
       </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C24" s="62"/>
-      <c r="D24" s="69" t="s">
+      <c r="C24" s="53"/>
+      <c r="D24" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E24" s="73">
+      <c r="E24" s="64">
         <v>47</v>
       </c>
-      <c r="F24" s="73" t="s">
+      <c r="F24" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="G24" s="74">
+      <c r="G24" s="65">
         <v>88555</v>
       </c>
-      <c r="H24" s="74">
+      <c r="H24" s="65">
         <v>92609</v>
       </c>
-      <c r="I24" s="74">
+      <c r="I24" s="65">
         <v>99988</v>
       </c>
-      <c r="J24" s="74">
+      <c r="J24" s="65">
         <v>101093</v>
       </c>
-      <c r="K24" s="74">
+      <c r="K24" s="65">
         <v>93091</v>
       </c>
-      <c r="L24" s="74">
+      <c r="L24" s="65">
         <v>82653</v>
       </c>
-      <c r="M24" s="74">
+      <c r="M24" s="65">
         <v>71252</v>
       </c>
-      <c r="N24" s="74" t="s">
+      <c r="N24" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="O24" s="74" t="s">
+      <c r="O24" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P24" s="65">
+      <c r="P24" s="56">
         <v>95361</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C25" s="62" t="s">
+      <c r="C25" s="53" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="69" t="s">
+      <c r="D25" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="73">
+      <c r="E25" s="64">
         <v>52</v>
       </c>
-      <c r="F25" s="73" t="s">
+      <c r="F25" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="74">
+      <c r="G25" s="65">
         <v>1645</v>
       </c>
-      <c r="H25" s="74">
+      <c r="H25" s="65">
         <v>3133</v>
       </c>
-      <c r="I25" s="74">
+      <c r="I25" s="65">
         <v>3383</v>
       </c>
-      <c r="J25" s="74">
+      <c r="J25" s="65">
         <v>2698</v>
       </c>
-      <c r="K25" s="74">
+      <c r="K25" s="65">
         <v>1870</v>
       </c>
-      <c r="L25" s="74">
+      <c r="L25" s="65">
         <v>1212</v>
       </c>
-      <c r="M25" s="74">
+      <c r="M25" s="65">
         <v>293</v>
       </c>
-      <c r="N25" s="74">
+      <c r="N25" s="65">
         <v>15</v>
       </c>
-      <c r="O25" s="74" t="s">
+      <c r="O25" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P25" s="65">
+      <c r="P25" s="56">
         <v>14249</v>
       </c>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C26" s="62"/>
-      <c r="D26" s="69" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="73">
+      <c r="E26" s="64">
         <v>52</v>
       </c>
-      <c r="F26" s="73" t="s">
+      <c r="F26" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="74">
+      <c r="G26" s="65">
         <v>91738</v>
       </c>
-      <c r="H26" s="74">
+      <c r="H26" s="65">
         <v>88111</v>
       </c>
-      <c r="I26" s="74">
+      <c r="I26" s="65">
         <v>95216</v>
       </c>
-      <c r="J26" s="74">
+      <c r="J26" s="65">
         <v>106204</v>
       </c>
-      <c r="K26" s="74">
+      <c r="K26" s="65">
         <v>111107</v>
       </c>
-      <c r="L26" s="74">
+      <c r="L26" s="65">
         <v>92436</v>
       </c>
-      <c r="M26" s="74">
+      <c r="M26" s="65">
         <v>90617</v>
       </c>
-      <c r="N26" s="74">
+      <c r="N26" s="65">
         <v>84431</v>
       </c>
-      <c r="O26" s="74" t="s">
+      <c r="O26" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="P26" s="65">
+      <c r="P26" s="56">
         <v>97076</v>
       </c>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C27" s="62" t="s">
+      <c r="C27" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="69" t="s">
+      <c r="D27" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="73">
+      <c r="E27" s="64">
         <v>57</v>
       </c>
-      <c r="F27" s="73" t="s">
+      <c r="F27" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="74">
+      <c r="G27" s="65">
         <v>1246</v>
       </c>
-      <c r="H27" s="74">
+      <c r="H27" s="65">
         <v>2369</v>
       </c>
-      <c r="I27" s="74">
+      <c r="I27" s="65">
         <v>2518</v>
       </c>
-      <c r="J27" s="74">
+      <c r="J27" s="65">
         <v>2321</v>
       </c>
-      <c r="K27" s="74">
+      <c r="K27" s="65">
         <v>1930</v>
       </c>
-      <c r="L27" s="74">
+      <c r="L27" s="65">
         <v>1820</v>
       </c>
-      <c r="M27" s="74">
+      <c r="M27" s="65">
         <v>903</v>
       </c>
-      <c r="N27" s="74">
+      <c r="N27" s="65">
         <v>269</v>
       </c>
-      <c r="O27" s="74">
+      <c r="O27" s="65">
         <v>3</v>
       </c>
-      <c r="P27" s="65">
+      <c r="P27" s="56">
         <v>13379</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C28" s="62"/>
-      <c r="D28" s="69" t="s">
+      <c r="C28" s="53"/>
+      <c r="D28" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="73">
+      <c r="E28" s="64">
         <v>57</v>
       </c>
-      <c r="F28" s="73" t="s">
+      <c r="F28" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="74">
+      <c r="G28" s="65">
         <v>93151</v>
       </c>
-      <c r="H28" s="74">
+      <c r="H28" s="65">
         <v>89757</v>
       </c>
-      <c r="I28" s="74">
+      <c r="I28" s="65">
         <v>94553</v>
       </c>
-      <c r="J28" s="74">
+      <c r="J28" s="65">
         <v>104728</v>
       </c>
-      <c r="K28" s="74">
+      <c r="K28" s="65">
         <v>119106</v>
       </c>
-      <c r="L28" s="74">
+      <c r="L28" s="65">
         <v>116131</v>
       </c>
-      <c r="M28" s="74">
+      <c r="M28" s="65">
         <v>104233</v>
       </c>
-      <c r="N28" s="74">
+      <c r="N28" s="65">
         <v>94529</v>
       </c>
-      <c r="O28" s="74">
+      <c r="O28" s="65">
         <v>86698</v>
       </c>
-      <c r="P28" s="65">
+      <c r="P28" s="56">
         <v>102467</v>
       </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C29" s="62" t="s">
+      <c r="C29" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="69" t="s">
+      <c r="D29" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="73">
+      <c r="E29" s="64">
         <v>62</v>
       </c>
-      <c r="F29" s="73" t="s">
+      <c r="F29" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="G29" s="74">
+      <c r="G29" s="65">
         <v>815</v>
       </c>
-      <c r="H29" s="74">
+      <c r="H29" s="65">
         <v>1571</v>
       </c>
-      <c r="I29" s="74">
+      <c r="I29" s="65">
         <v>1710</v>
       </c>
-      <c r="J29" s="74">
+      <c r="J29" s="65">
         <v>1396</v>
       </c>
-      <c r="K29" s="74">
+      <c r="K29" s="65">
         <v>1096</v>
       </c>
-      <c r="L29" s="74">
+      <c r="L29" s="65">
         <v>1095</v>
       </c>
-      <c r="M29" s="74">
+      <c r="M29" s="65">
         <v>626</v>
       </c>
-      <c r="N29" s="74">
+      <c r="N29" s="65">
         <v>245</v>
       </c>
-      <c r="O29" s="74">
+      <c r="O29" s="65">
         <v>28</v>
       </c>
-      <c r="P29" s="65">
+      <c r="P29" s="56">
         <v>8582</v>
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C30" s="62"/>
-      <c r="D30" s="69" t="s">
+      <c r="C30" s="53"/>
+      <c r="D30" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="73">
+      <c r="E30" s="64">
         <v>62</v>
       </c>
-      <c r="F30" s="73" t="s">
+      <c r="F30" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="74">
+      <c r="G30" s="65">
         <v>99546</v>
       </c>
-      <c r="H30" s="74">
+      <c r="H30" s="65">
         <v>93632</v>
       </c>
-      <c r="I30" s="74">
+      <c r="I30" s="65">
         <v>96989</v>
       </c>
-      <c r="J30" s="74">
+      <c r="J30" s="65">
         <v>105313</v>
       </c>
-      <c r="K30" s="74">
+      <c r="K30" s="65">
         <v>123261</v>
       </c>
-      <c r="L30" s="74">
+      <c r="L30" s="65">
         <v>131919</v>
       </c>
-      <c r="M30" s="74">
+      <c r="M30" s="65">
         <v>148713</v>
       </c>
-      <c r="N30" s="74">
+      <c r="N30" s="65">
         <v>115391</v>
       </c>
-      <c r="O30" s="74">
+      <c r="O30" s="65">
         <v>108176</v>
       </c>
-      <c r="P30" s="65">
+      <c r="P30" s="56">
         <v>110118</v>
       </c>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="69" t="s">
+      <c r="D31" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="73">
+      <c r="E31" s="64">
         <v>67</v>
       </c>
-      <c r="F31" s="73" t="s">
+      <c r="F31" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="G31" s="74">
+      <c r="G31" s="65">
         <v>268</v>
       </c>
-      <c r="H31" s="74">
+      <c r="H31" s="65">
         <v>610</v>
       </c>
-      <c r="I31" s="74">
+      <c r="I31" s="65">
         <v>613</v>
       </c>
-      <c r="J31" s="74">
+      <c r="J31" s="65">
         <v>480</v>
       </c>
-      <c r="K31" s="74">
+      <c r="K31" s="65">
         <v>380</v>
       </c>
-      <c r="L31" s="74">
+      <c r="L31" s="65">
         <v>351</v>
       </c>
-      <c r="M31" s="74">
+      <c r="M31" s="65">
         <v>295</v>
       </c>
-      <c r="N31" s="74">
+      <c r="N31" s="65">
         <v>224</v>
       </c>
-      <c r="O31" s="74">
+      <c r="O31" s="65">
         <v>70</v>
       </c>
-      <c r="P31" s="65">
+      <c r="P31" s="56">
         <v>3291</v>
       </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C32" s="62"/>
-      <c r="D32" s="69" t="s">
+      <c r="C32" s="53"/>
+      <c r="D32" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="73">
+      <c r="E32" s="64">
         <v>67</v>
       </c>
-      <c r="F32" s="73" t="s">
+      <c r="F32" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="G32" s="74">
+      <c r="G32" s="65">
         <v>109046</v>
       </c>
-      <c r="H32" s="74">
+      <c r="H32" s="65">
         <v>100493</v>
       </c>
-      <c r="I32" s="74">
+      <c r="I32" s="65">
         <v>111602</v>
       </c>
-      <c r="J32" s="74">
+      <c r="J32" s="65">
         <v>112632</v>
       </c>
-      <c r="K32" s="74">
+      <c r="K32" s="65">
         <v>134768</v>
       </c>
-      <c r="L32" s="74">
+      <c r="L32" s="65">
         <v>147005</v>
       </c>
-      <c r="M32" s="74">
+      <c r="M32" s="65">
         <v>167347</v>
       </c>
-      <c r="N32" s="74">
+      <c r="N32" s="65">
         <v>186061</v>
       </c>
-      <c r="O32" s="74">
+      <c r="O32" s="65">
         <v>176875</v>
       </c>
-      <c r="P32" s="65">
+      <c r="P32" s="56">
         <v>127389</v>
       </c>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C33" s="62" t="s">
+      <c r="C33" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="69" t="s">
+      <c r="D33" s="60" t="s">
         <v>109</v>
       </c>
-      <c r="E33" s="73">
+      <c r="E33" s="64">
         <v>72</v>
       </c>
-      <c r="F33" s="73" t="s">
+      <c r="F33" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="G33" s="74">
+      <c r="G33" s="65">
         <v>132</v>
       </c>
-      <c r="H33" s="74">
+      <c r="H33" s="65">
         <v>164</v>
       </c>
-      <c r="I33" s="74">
+      <c r="I33" s="65">
         <v>172</v>
       </c>
-      <c r="J33" s="74">
+      <c r="J33" s="65">
         <v>141</v>
       </c>
-      <c r="K33" s="74">
+      <c r="K33" s="65">
         <v>121</v>
       </c>
-      <c r="L33" s="74">
+      <c r="L33" s="65">
         <v>133</v>
       </c>
-      <c r="M33" s="74">
+      <c r="M33" s="65">
         <v>115</v>
       </c>
-      <c r="N33" s="74">
+      <c r="N33" s="65">
         <v>141</v>
       </c>
-      <c r="O33" s="74">
+      <c r="O33" s="65">
         <v>218</v>
       </c>
-      <c r="P33" s="65">
+      <c r="P33" s="56">
         <v>1337</v>
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C34" s="62"/>
-      <c r="D34" s="69" t="s">
+      <c r="C34" s="53"/>
+      <c r="D34" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="E34" s="73">
+      <c r="E34" s="64">
         <v>72</v>
       </c>
-      <c r="F34" s="73" t="s">
+      <c r="F34" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="G34" s="74">
+      <c r="G34" s="65">
         <v>120037</v>
       </c>
-      <c r="H34" s="74">
+      <c r="H34" s="65">
         <v>120246</v>
       </c>
-      <c r="I34" s="74">
+      <c r="I34" s="65">
         <v>133740</v>
       </c>
-      <c r="J34" s="74">
+      <c r="J34" s="65">
         <v>152829</v>
       </c>
-      <c r="K34" s="74">
+      <c r="K34" s="65">
         <v>158421</v>
       </c>
-      <c r="L34" s="74">
+      <c r="L34" s="65">
         <v>182235</v>
       </c>
-      <c r="M34" s="74">
+      <c r="M34" s="65">
         <v>198905</v>
       </c>
-      <c r="N34" s="74">
+      <c r="N34" s="65">
         <v>201823</v>
       </c>
-      <c r="O34" s="74">
+      <c r="O34" s="65">
         <v>199972</v>
       </c>
-      <c r="P34" s="65">
+      <c r="P34" s="56">
         <v>163387</v>
       </c>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C35" s="62" t="s">
+      <c r="C35" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="60" t="s">
+      <c r="D35" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="F35" s="72" t="s">
+      <c r="F35" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="G35" s="65">
+      <c r="G35" s="56">
         <v>22401</v>
       </c>
-      <c r="H35" s="65">
+      <c r="H35" s="56">
         <v>27903</v>
       </c>
-      <c r="I35" s="65">
+      <c r="I35" s="56">
         <v>19244</v>
       </c>
-      <c r="J35" s="65">
+      <c r="J35" s="56">
         <v>11568</v>
       </c>
-      <c r="K35" s="65">
+      <c r="K35" s="56">
         <v>6739</v>
       </c>
-      <c r="L35" s="65">
+      <c r="L35" s="56">
         <v>4967</v>
       </c>
-      <c r="M35" s="65">
+      <c r="M35" s="56">
         <v>2243</v>
       </c>
-      <c r="N35" s="62">
+      <c r="N35" s="53">
         <v>894</v>
       </c>
-      <c r="O35" s="62">
+      <c r="O35" s="53">
         <v>319</v>
       </c>
-      <c r="P35" s="65">
+      <c r="P35" s="56">
         <v>96278</v>
       </c>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C36" s="58"/>
-      <c r="D36" s="60" t="s">
+      <c r="C36" s="50"/>
+      <c r="D36" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="F36" s="72" t="s">
+      <c r="F36" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="G36" s="64">
+      <c r="G36" s="55">
         <v>82337</v>
       </c>
-      <c r="H36" s="64">
+      <c r="H36" s="55">
         <v>88439</v>
       </c>
-      <c r="I36" s="64">
+      <c r="I36" s="55">
         <v>93978</v>
       </c>
-      <c r="J36" s="64">
+      <c r="J36" s="55">
         <v>101272</v>
       </c>
-      <c r="K36" s="64">
+      <c r="K36" s="55">
         <v>113443</v>
       </c>
-      <c r="L36" s="64">
+      <c r="L36" s="55">
         <v>115372</v>
       </c>
-      <c r="M36" s="64">
+      <c r="M36" s="55">
         <v>127861</v>
       </c>
-      <c r="N36" s="64">
+      <c r="N36" s="55">
         <v>139933</v>
       </c>
-      <c r="O36" s="64">
+      <c r="O36" s="55">
         <v>185781</v>
       </c>
-      <c r="P36" s="64">
+      <c r="P36" s="55">
         <v>94527</v>
       </c>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C37" s="59"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="66"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="59"/>
+      <c r="C37" s="51"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="57"/>
+      <c r="I37" s="57"/>
+      <c r="J37" s="57"/>
+      <c r="K37" s="57"/>
+      <c r="L37" s="57"/>
+      <c r="M37" s="57"/>
+      <c r="N37" s="57"/>
+      <c r="O37" s="57"/>
+      <c r="P37" s="51"/>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C38" s="59"/>
-      <c r="G38" s="66"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="59"/>
-      <c r="N38" s="59"/>
-      <c r="O38" s="59"/>
-      <c r="P38" s="59"/>
+      <c r="C38" s="51"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="M38" s="51"/>
+      <c r="N38" s="51"/>
+      <c r="O38" s="51"/>
+      <c r="P38" s="51"/>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C39" s="59"/>
-      <c r="G39" s="71"/>
-      <c r="H39" s="71"/>
-      <c r="I39" s="71"/>
-      <c r="J39" s="71"/>
-      <c r="K39" s="71"/>
-      <c r="L39" s="71"/>
-      <c r="M39" s="71"/>
-      <c r="N39" s="71"/>
-      <c r="O39" s="71"/>
-      <c r="P39" s="59"/>
+      <c r="C39" s="51"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="62"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="62"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="62"/>
+      <c r="P39" s="51"/>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="59"/>
-      <c r="M40" s="59"/>
-      <c r="N40" s="59"/>
-      <c r="O40" s="59"/>
-      <c r="P40" s="59"/>
+      <c r="C40" s="51"/>
+      <c r="G40" s="51"/>
+      <c r="H40" s="51"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="51"/>
+      <c r="O40" s="51"/>
+      <c r="P40" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4516,17 +4996,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4545,26 +5025,26 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
@@ -4575,18 +5055,18 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
       <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4595,10 +5075,10 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -5487,17 +5967,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5516,26 +5996,26 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="54"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
@@ -5546,18 +6026,18 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="52"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68"/>
       <c r="K5" s="37"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5581,10 +6061,10 @@
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="52"/>
+      <c r="G7" s="68"/>
       <c r="H7" s="37"/>
       <c r="I7" s="37"/>
       <c r="J7" s="37"/>
@@ -6475,17 +6955,17 @@
       <c r="A1" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="52"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="68"/>
       <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6504,25 +6984,25 @@
       <c r="K2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
     </row>
     <row r="4" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="54"/>
+      <c r="B4" s="70"/>
       <c r="C4" s="38"/>
       <c r="D4" s="38"/>
       <c r="E4" s="38"/>
@@ -6534,10 +7014,10 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="52"/>
+      <c r="B5" s="68"/>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
@@ -6554,10 +7034,10 @@
       <c r="C6" s="38"/>
       <c r="D6" s="38"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="53" t="s">
+      <c r="F6" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="54"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="38"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38"/>
@@ -7847,12 +8327,12 @@
     </row>
     <row r="35" spans="1:6" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="56"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -8084,12 +8564,12 @@
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="22"/>
-      <c r="B51" s="56" t="s">
+      <c r="B51" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="72"/>
+      <c r="E51" s="72"/>
     </row>
     <row r="52" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
@@ -8279,12 +8759,12 @@
     </row>
     <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="22"/>
-      <c r="B68" s="56" t="s">
+      <c r="B68" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C68" s="56"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="56"/>
+      <c r="C68" s="72"/>
+      <c r="D68" s="72"/>
+      <c r="E68" s="72"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
@@ -8393,12 +8873,12 @@
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
-      <c r="B78" s="56" t="s">
+      <c r="B78" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C78" s="56"/>
-      <c r="D78" s="56"/>
-      <c r="E78" s="56"/>
+      <c r="C78" s="72"/>
+      <c r="D78" s="72"/>
+      <c r="E78" s="72"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="17" t="s">
@@ -8650,7 +9130,7 @@
       <c r="J101" s="12"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A102" s="55" t="s">
+      <c r="A102" s="71" t="s">
         <v>65</v>
       </c>
       <c r="B102" s="6" t="s">
@@ -8676,7 +9156,7 @@
       <c r="J102" s="12"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="55"/>
+      <c r="A103" s="71"/>
       <c r="B103" s="6" t="s">
         <v>12</v>
       </c>
@@ -8700,7 +9180,7 @@
       <c r="J103" s="12"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A104" s="55" t="s">
+      <c r="A104" s="71" t="s">
         <v>13</v>
       </c>
       <c r="B104" s="6" t="s">
@@ -8726,7 +9206,7 @@
       <c r="J104" s="12"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A105" s="55"/>
+      <c r="A105" s="71"/>
       <c r="B105" s="6" t="s">
         <v>12</v>
       </c>
@@ -8750,7 +9230,7 @@
       <c r="J105" s="12"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A106" s="55" t="s">
+      <c r="A106" s="71" t="s">
         <v>14</v>
       </c>
       <c r="B106" s="6" t="s">
@@ -8776,7 +9256,7 @@
       <c r="J106" s="12"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A107" s="55"/>
+      <c r="A107" s="71"/>
       <c r="B107" s="6" t="s">
         <v>12</v>
       </c>
@@ -9527,12 +10007,12 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -9679,12 +10159,12 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="22"/>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">

</xml_diff>

<commit_message>
update run control file for return scenarios
</commit_message>
<xml_diff>
--- a/Data/UCRP-MembersData-2015(1).xlsx
+++ b/Data/UCRP-MembersData-2015(1).xlsx
@@ -9,34 +9,35 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900"/>
   </bookViews>
   <sheets>
-    <sheet name="Data_Doc" sheetId="2" r:id="rId1"/>
-    <sheet name="2015" sheetId="4" r:id="rId2"/>
-    <sheet name="Sum_Disabled" sheetId="19" r:id="rId3"/>
-    <sheet name="Sum_Retirees" sheetId="20" r:id="rId4"/>
-    <sheet name="Sum_Active" sheetId="18" r:id="rId5"/>
-    <sheet name="CAP" sheetId="17" r:id="rId6"/>
-    <sheet name="Disabled_Inc" sheetId="15" r:id="rId7"/>
-    <sheet name="Disabled_HAPC" sheetId="16" r:id="rId8"/>
-    <sheet name="Terms_N_t76_raw" sheetId="13" r:id="rId9"/>
-    <sheet name="Terms_HAPC_t76_raw" sheetId="14" r:id="rId10"/>
-    <sheet name="Retirees_t76" sheetId="11" r:id="rId11"/>
-    <sheet name="Beneficiaries_t76" sheetId="12" r:id="rId12"/>
-    <sheet name="Actives_t76" sheetId="7" r:id="rId13"/>
-    <sheet name="Actives_t13" sheetId="22" r:id="rId14"/>
-    <sheet name="Actives_tm13" sheetId="23" r:id="rId15"/>
-    <sheet name="Actives_t13_raw" sheetId="8" r:id="rId16"/>
-    <sheet name="Actives_tm13_raw" sheetId="9" r:id="rId17"/>
-    <sheet name="Actives_safety" sheetId="10" r:id="rId18"/>
+    <sheet name="TOC" sheetId="24" r:id="rId1"/>
+    <sheet name="Data_Doc" sheetId="2" r:id="rId2"/>
+    <sheet name="2015" sheetId="4" r:id="rId3"/>
+    <sheet name="Sum_Disabled" sheetId="19" r:id="rId4"/>
+    <sheet name="Sum_Retirees" sheetId="20" r:id="rId5"/>
+    <sheet name="Sum_Active" sheetId="18" r:id="rId6"/>
+    <sheet name="CAP" sheetId="17" r:id="rId7"/>
+    <sheet name="Disabled_Inc" sheetId="15" r:id="rId8"/>
+    <sheet name="Disabled_HAPC" sheetId="16" r:id="rId9"/>
+    <sheet name="Terms_N_t76_raw" sheetId="13" r:id="rId10"/>
+    <sheet name="Terms_HAPC_t76_raw" sheetId="14" r:id="rId11"/>
+    <sheet name="Retirees_t76" sheetId="11" r:id="rId12"/>
+    <sheet name="Beneficiaries_t76" sheetId="12" r:id="rId13"/>
+    <sheet name="Actives_t76" sheetId="7" r:id="rId14"/>
+    <sheet name="Actives_t13" sheetId="22" r:id="rId15"/>
+    <sheet name="Actives_tm13" sheetId="23" r:id="rId16"/>
+    <sheet name="Actives_t13_raw" sheetId="8" r:id="rId17"/>
+    <sheet name="Actives_tm13_raw" sheetId="9" r:id="rId18"/>
+    <sheet name="Actives_safety" sheetId="10" r:id="rId19"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="181">
   <si>
     <t>&lt; 50</t>
   </si>
@@ -513,6 +514,117 @@
   <si>
     <t>Data in the black frame must be of the type of "Number"</t>
   </si>
+  <si>
+    <t>Sheet #</t>
+  </si>
+  <si>
+    <t>Table of Contents</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Data_Doc</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Sum_Disabled</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Sum_Retirees</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Sum_Active</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Disabled_Inc</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Disabled_HAPC</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Terms_N_t76_raw</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Terms_HAPC_t76_raw</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Retirees_t76</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Beneficiaries_t76</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Actives_t76</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Actives_t13</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Actives_tm13</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Actives_t13_raw</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Actives_tm13_raw</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Actives_safety</t>
+  </si>
 </sst>
 </file>
 
@@ -524,7 +636,7 @@
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +718,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -799,10 +919,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1075,8 +1196,11 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1413,46 +1537,477 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>67</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="100" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="101" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="100" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="101">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="100" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="100" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="101" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="100" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="101" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="100" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="101" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="100" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="101" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="100" t="s">
+        <v>159</v>
+      </c>
+      <c r="B9" s="101" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="100" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="101" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="100" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="101" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="100" t="s">
+        <v>165</v>
+      </c>
+      <c r="B12" s="101" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="100" t="s">
+        <v>167</v>
+      </c>
+      <c r="B13" s="101" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="100" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" s="101" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="100" t="s">
+        <v>171</v>
+      </c>
+      <c r="B15" s="101" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="100" t="s">
+        <v>173</v>
+      </c>
+      <c r="B16" s="101" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="100" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="101" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="100" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="101" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="100" t="s">
+        <v>179</v>
+      </c>
+      <c r="B19" s="101" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" location="'Data_Doc'!A1" display="Data_Doc"/>
+    <hyperlink ref="B3" location="'2015'!A1" display="2015"/>
+    <hyperlink ref="B4" location="'Sum_Disabled'!A1" display="Sum_Disabled"/>
+    <hyperlink ref="B5" location="'Sum_Retirees'!A1" display="Sum_Retirees"/>
+    <hyperlink ref="B6" location="'Sum_Active'!A1" display="Sum_Active"/>
+    <hyperlink ref="B7" location="'CAP'!A1" display="CAP"/>
+    <hyperlink ref="B8" location="'Disabled_Inc'!A1" display="Disabled_Inc"/>
+    <hyperlink ref="B9" location="'Disabled_HAPC'!A1" display="Disabled_HAPC"/>
+    <hyperlink ref="B10" location="'Terms_N_t76_raw'!A1" display="Terms_N_t76_raw"/>
+    <hyperlink ref="B11" location="'Terms_HAPC_t76_raw'!A1" display="Terms_HAPC_t76_raw"/>
+    <hyperlink ref="B12" location="'Retirees_t76'!A1" display="Retirees_t76"/>
+    <hyperlink ref="B13" location="'Beneficiaries_t76'!A1" display="Beneficiaries_t76"/>
+    <hyperlink ref="B14" location="'Actives_t76'!A1" display="Actives_t76"/>
+    <hyperlink ref="B15" location="'Actives_t13'!A1" display="Actives_t13"/>
+    <hyperlink ref="B16" location="'Actives_tm13'!A1" display="Actives_tm13"/>
+    <hyperlink ref="B17" location="'Actives_t13_raw'!A1" display="Actives_t13_raw"/>
+    <hyperlink ref="B18" location="'Actives_tm13_raw'!A1" display="Actives_tm13_raw"/>
+    <hyperlink ref="B19" location="'Actives_safety'!A1" display="Actives_safety"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="92" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="25">
+        <v>1024</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="26">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="25">
+        <v>7321</v>
+      </c>
+      <c r="C8" s="25">
+        <v>204</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="26">
+        <v>7525</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="25">
+        <v>8546</v>
+      </c>
+      <c r="C9" s="25">
+        <v>2041</v>
+      </c>
+      <c r="D9" s="25">
+        <v>42</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="26">
+        <v>10629</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="25">
+        <v>4315</v>
+      </c>
+      <c r="C10" s="25">
+        <v>2542</v>
+      </c>
+      <c r="D10" s="25">
+        <v>183</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="26">
+        <v>7040</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="25">
+        <v>3409</v>
+      </c>
+      <c r="C11" s="25">
+        <v>3981</v>
+      </c>
+      <c r="D11" s="25">
+        <v>493</v>
+      </c>
+      <c r="E11" s="25">
+        <v>2</v>
+      </c>
+      <c r="F11" s="26">
+        <v>7885</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="25">
+        <v>2440</v>
+      </c>
+      <c r="C12" s="25">
+        <v>4933</v>
+      </c>
+      <c r="D12" s="25">
+        <v>954</v>
+      </c>
+      <c r="E12" s="25">
+        <v>45</v>
+      </c>
+      <c r="F12" s="26">
+        <v>8372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="25">
+        <v>2286</v>
+      </c>
+      <c r="C13" s="25">
+        <v>4901</v>
+      </c>
+      <c r="D13" s="25">
+        <v>1330</v>
+      </c>
+      <c r="E13" s="25">
+        <v>82</v>
+      </c>
+      <c r="F13" s="26">
+        <v>8599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="25">
+        <v>1997</v>
+      </c>
+      <c r="C14" s="25">
+        <v>4034</v>
+      </c>
+      <c r="D14" s="25">
+        <v>1183</v>
+      </c>
+      <c r="E14" s="25">
+        <v>93</v>
+      </c>
+      <c r="F14" s="26">
+        <v>7307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="25">
+        <v>2902</v>
+      </c>
+      <c r="C15" s="25">
+        <v>1892</v>
+      </c>
+      <c r="D15" s="25">
+        <v>400</v>
+      </c>
+      <c r="E15" s="25">
+        <v>39</v>
+      </c>
+      <c r="F15" s="26">
+        <v>5233</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="26">
+        <v>34240</v>
+      </c>
+      <c r="C16" s="26">
+        <v>24528</v>
+      </c>
+      <c r="D16" s="26">
+        <v>4585</v>
+      </c>
+      <c r="E16" s="26">
+        <v>261</v>
+      </c>
+      <c r="F16" s="26">
+        <v>63614</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -1659,7 +2214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
@@ -2004,7 +2559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -2299,7 +2854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P40"/>
   <sheetViews>
@@ -3602,7 +4157,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P40"/>
   <sheetViews>
@@ -4883,7 +5438,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P40"/>
   <sheetViews>
@@ -6090,7 +6645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -7061,7 +7616,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
@@ -8047,7 +8602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K31"/>
   <sheetViews>
@@ -9022,9 +9577,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J122"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
@@ -10602,7 +11198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -10659,7 +11255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -10758,7 +11354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -10948,7 +11544,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -11052,7 +11648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -11195,7 +11791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -11345,282 +11941,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G75" sqref="G75"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="92" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="47" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="25">
-        <v>1024</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="26">
-        <v>1024</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="25">
-        <v>7321</v>
-      </c>
-      <c r="C8" s="25">
-        <v>204</v>
-      </c>
-      <c r="D8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="26">
-        <v>7525</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" s="25">
-        <v>8546</v>
-      </c>
-      <c r="C9" s="25">
-        <v>2041</v>
-      </c>
-      <c r="D9" s="25">
-        <v>42</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="26">
-        <v>10629</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B10" s="25">
-        <v>4315</v>
-      </c>
-      <c r="C10" s="25">
-        <v>2542</v>
-      </c>
-      <c r="D10" s="25">
-        <v>183</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="26">
-        <v>7040</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="25">
-        <v>3409</v>
-      </c>
-      <c r="C11" s="25">
-        <v>3981</v>
-      </c>
-      <c r="D11" s="25">
-        <v>493</v>
-      </c>
-      <c r="E11" s="25">
-        <v>2</v>
-      </c>
-      <c r="F11" s="26">
-        <v>7885</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="25">
-        <v>2440</v>
-      </c>
-      <c r="C12" s="25">
-        <v>4933</v>
-      </c>
-      <c r="D12" s="25">
-        <v>954</v>
-      </c>
-      <c r="E12" s="25">
-        <v>45</v>
-      </c>
-      <c r="F12" s="26">
-        <v>8372</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="25">
-        <v>2286</v>
-      </c>
-      <c r="C13" s="25">
-        <v>4901</v>
-      </c>
-      <c r="D13" s="25">
-        <v>1330</v>
-      </c>
-      <c r="E13" s="25">
-        <v>82</v>
-      </c>
-      <c r="F13" s="26">
-        <v>8599</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="25">
-        <v>1997</v>
-      </c>
-      <c r="C14" s="25">
-        <v>4034</v>
-      </c>
-      <c r="D14" s="25">
-        <v>1183</v>
-      </c>
-      <c r="E14" s="25">
-        <v>93</v>
-      </c>
-      <c r="F14" s="26">
-        <v>7307</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="25">
-        <v>2902</v>
-      </c>
-      <c r="C15" s="25">
-        <v>1892</v>
-      </c>
-      <c r="D15" s="25">
-        <v>400</v>
-      </c>
-      <c r="E15" s="25">
-        <v>39</v>
-      </c>
-      <c r="F15" s="26">
-        <v>5233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="26">
-        <v>34240</v>
-      </c>
-      <c r="C16" s="26">
-        <v>24528</v>
-      </c>
-      <c r="D16" s="26">
-        <v>4585</v>
-      </c>
-      <c r="E16" s="26">
-        <v>261</v>
-      </c>
-      <c r="F16" s="26">
-        <v>63614</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B5:E5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>